<commit_message>
Change title event for tasks, full workTime slot...
</commit_message>
<xml_diff>
--- a/Templates/Store_template.xlsx
+++ b/Templates/Store_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksandar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Koj@_project\Customer Management\custom_management\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>street</t>
   </si>
@@ -66,16 +66,45 @@
   </si>
   <si>
     <t>store21</t>
+  </si>
+  <si>
+    <t>store21@gmail.com</t>
+  </si>
+  <si>
+    <t>066/44564545</t>
+  </si>
+  <si>
+    <t>035/44565454</t>
+  </si>
+  <si>
+    <t>No comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Tue Aug 13 2019 07:00:00 GMT+0200 (Central European Summer Time)</t>
+  </si>
+  <si>
+    <t>Tue Aug 13 2019 14:00:00 GMT+0200 (Central European Summer Time)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,14 +133,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,11 +437,11 @@
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
@@ -454,48 +489,51 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>45</v>
+      </c>
+      <c r="L2">
+        <v>15</v>
       </c>
       <c r="M2">
         <v>85</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>